<commit_message>
Update meta data retreival for ipx conversion
</commit_message>
<xml_diff>
--- a/ir_tools/data_formats/meta_data_record/Record_of_MWIR1_FLIR_SC7500_6580045_Operating_Settings.xlsx
+++ b/ir_tools/data_formats/meta_data_record/Record_of_MWIR1_FLIR_SC7500_6580045_Operating_Settings.xlsx
@@ -484,28 +484,28 @@
   <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B9" xSplit="1" ySplit="5"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="B6" xSplit="1" ySplit="5"/>
       <selection activeCell="B1" pane="topRight" sqref="B1"/>
       <selection activeCell="A6" pane="bottomLeft" sqref="A6"/>
-      <selection activeCell="L13" pane="bottomRight" sqref="L13:N13"/>
+      <selection activeCell="C8" pane="bottomRight" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="9" width="12.7109375"/>
-    <col customWidth="1" max="2" min="2" style="5" width="11.28515625"/>
-    <col customWidth="1" max="3" min="3" style="9" width="10.85546875"/>
-    <col customWidth="1" max="4" min="4" style="9" width="10.42578125"/>
-    <col customWidth="1" max="5" min="5" style="9" width="11.5703125"/>
-    <col customWidth="1" max="6" min="6" style="9" width="8.7109375"/>
-    <col customWidth="1" max="7" min="7" style="9" width="8.28515625"/>
-    <col customWidth="1" max="8" min="8" style="9" width="7.28515625"/>
+    <col customWidth="1" max="1" min="1" style="9" width="12.6640625"/>
+    <col customWidth="1" max="2" min="2" style="5" width="11.33203125"/>
+    <col customWidth="1" max="3" min="3" style="9" width="10.88671875"/>
+    <col customWidth="1" max="4" min="4" style="9" width="10.44140625"/>
+    <col customWidth="1" max="5" min="5" style="9" width="11.5546875"/>
+    <col customWidth="1" max="6" min="6" style="9" width="8.6640625"/>
+    <col customWidth="1" max="7" min="7" style="9" width="8.33203125"/>
+    <col customWidth="1" max="8" min="8" style="9" width="7.33203125"/>
     <col customWidth="1" max="9" min="9" style="5" width="22"/>
     <col bestFit="1" customWidth="1" max="10" min="10" style="5" width="10"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="5" width="18.85546875"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="5" width="9.28515625"/>
-    <col customWidth="1" max="13" min="13" style="5" width="38.42578125"/>
-    <col customWidth="1" max="14" min="14" style="5" width="82.140625"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="5" width="18.88671875"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="5" width="9.33203125"/>
+    <col customWidth="1" max="13" min="13" style="5" width="38.44140625"/>
+    <col customWidth="1" max="14" min="14" style="5" width="82.109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -558,7 +558,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="28.9" r="5" s="4">
+    <row customFormat="1" customHeight="1" ht="28.95" r="5" s="4">
       <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Shot</t>
@@ -571,7 +571,7 @@
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Integration time [ms]</t>
+          <t>Integration time [us]</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">
@@ -638,7 +638,7 @@
         <v>44328</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001</v>
+        <v>100</v>
       </c>
       <c r="D6" t="n">
         <v>382.00015280006</v>
@@ -696,7 +696,7 @@
         <v>44328</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D7" t="n">
         <v>382.00015280006</v>
@@ -753,8 +753,8 @@
       <c r="B8" s="2" t="n">
         <v>44328</v>
       </c>
-      <c r="C8" s="3" t="n">
-        <v>0.001</v>
+      <c r="C8" t="n">
+        <v>100</v>
       </c>
       <c r="D8" t="n">
         <v>382.00015280006</v>
@@ -811,8 +811,8 @@
       <c r="B9" s="2" t="n">
         <v>44328</v>
       </c>
-      <c r="C9" s="3" t="n">
-        <v>0.001</v>
+      <c r="C9" t="n">
+        <v>100</v>
       </c>
       <c r="D9" t="n">
         <v>382.00015280006</v>
@@ -869,8 +869,8 @@
       <c r="B10" s="2" t="n">
         <v>44329</v>
       </c>
-      <c r="C10" s="3" t="n">
-        <v>0.001</v>
+      <c r="C10" t="n">
+        <v>100</v>
       </c>
       <c r="D10" t="n">
         <v>382.00015280006</v>
@@ -927,8 +927,8 @@
       <c r="B11" s="2" t="n">
         <v>44329</v>
       </c>
-      <c r="C11" s="3" t="n">
-        <v>0.001</v>
+      <c r="C11" t="n">
+        <v>100</v>
       </c>
       <c r="D11" t="n">
         <v>382.00015280006</v>
@@ -986,7 +986,7 @@
         <v>44329</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>0.001</v>
+        <v>300</v>
       </c>
       <c r="D12" t="n">
         <v>382.00015280006</v>

</xml_diff>